<commit_message>
Updated experiment on ck
</commit_message>
<xml_diff>
--- a/Parameters-Estimation/Ck_Parameters_Estimation/1-Trained-Models/training_test_2016_2019/Results-ck-test-model.xlsx
+++ b/Parameters-Estimation/Ck_Parameters_Estimation/1-Trained-Models/training_test_2016_2019/Results-ck-test-model.xlsx
@@ -142,28 +142,28 @@
         <v>1</v>
       </c>
       <c r="B2" s="0">
-        <v>52.501687931789846</v>
+        <v>45.6773314456603</v>
       </c>
       <c r="C2" s="0">
-        <v>0.42722544312682437</v>
+        <v>0.40873237147177988</v>
       </c>
       <c r="D2" s="0">
-        <v>35.181616473598964</v>
+        <v>32.042792113907446</v>
       </c>
       <c r="E2" s="0">
-        <v>0.37466418163723542</v>
+        <v>0.28845639571382869</v>
       </c>
       <c r="F2" s="0">
-        <v>0.61209817973690739</v>
+        <v>0.53708136787066885</v>
       </c>
       <c r="G2" s="0">
-        <v>0.57593460835466503</v>
+        <v>0.50649466706193247</v>
       </c>
       <c r="H2" s="0">
-        <v>0.62533581836276464</v>
+        <v>0.71154360428617136</v>
       </c>
       <c r="I2" s="0">
-        <v>0.79567731914863637</v>
+        <v>0.84719231370516268</v>
       </c>
     </row>
     <row r="3">
@@ -171,28 +171,28 @@
         <v>2</v>
       </c>
       <c r="B3" s="0">
-        <v>51.325481977737184</v>
+        <v>47.126364750062592</v>
       </c>
       <c r="C3" s="0">
-        <v>0.41765422494844101</v>
+        <v>0.42169868977683511</v>
       </c>
       <c r="D3" s="0">
-        <v>34.81758932365662</v>
+        <v>33.086163228014279</v>
       </c>
       <c r="E3" s="0">
-        <v>0.35806487172545992</v>
+        <v>0.30704823541900106</v>
       </c>
       <c r="F3" s="0">
-        <v>0.59838522017631746</v>
+        <v>0.55411933319367324</v>
       </c>
       <c r="G3" s="0">
-        <v>0.56997536443561891</v>
+        <v>0.52298704710119293</v>
       </c>
       <c r="H3" s="0">
-        <v>0.64193512827454002</v>
+        <v>0.69295176458099894</v>
       </c>
       <c r="I3" s="0">
-        <v>0.80688578970048619</v>
+        <v>0.83288058624949202</v>
       </c>
     </row>
     <row r="4">
@@ -200,28 +200,28 @@
         <v>3</v>
       </c>
       <c r="B4" s="0">
-        <v>52.926525701934615</v>
+        <v>48.388797894883567</v>
       </c>
       <c r="C4" s="0">
-        <v>0.43068250349491993</v>
+        <v>0.43299526242624886</v>
       </c>
       <c r="D4" s="0">
-        <v>36.224496806703975</v>
+        <v>35.178524982019304</v>
       </c>
       <c r="E4" s="0">
-        <v>0.38075219521241299</v>
+        <v>0.32371915026352605</v>
       </c>
       <c r="F4" s="0">
-        <v>0.6170512095542906</v>
+        <v>0.56896322399916677</v>
       </c>
       <c r="G4" s="0">
-        <v>0.59300690168315218</v>
+        <v>0.55606063401585903</v>
       </c>
       <c r="H4" s="0">
-        <v>0.61924780478758701</v>
+        <v>0.67628084973647395</v>
       </c>
       <c r="I4" s="0">
-        <v>0.7911519297966646</v>
+        <v>0.83429447792900602</v>
       </c>
     </row>
   </sheetData>

</xml_diff>